<commit_message>
Fix base url to be complete
</commit_message>
<xml_diff>
--- a/PaladinEcomAPITestStore.xlsx
+++ b/PaladinEcomAPITestStore.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3D84DA-C963-448A-8E85-499BB52AF1F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA34055-7704-4ACF-B447-BBE652D712CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24540" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43635" yWindow="2760" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Description1</t>
   </si>
   <si>
-    <t>https://mobile2.paladinpos.com</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Paladin Ecom API Documentation available at</t>
   </si>
   <si>
-    <t>https://github.com/PaladinPOS</t>
-  </si>
-  <si>
     <t>CLEANR PANEL LQ GOLD16OZ</t>
   </si>
   <si>
@@ -377,13 +371,19 @@
   </si>
   <si>
     <t>Some example data that exist in the test store database:</t>
+  </si>
+  <si>
+    <t>https://mobile2.paladinpos.com/api/v1/pos</t>
+  </si>
+  <si>
+    <t>https://github.com/PaladinPOS/PaladinEcomAPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +395,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -417,10 +425,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -429,8 +438,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -712,7 +724,7 @@
   <dimension ref="A2:W68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,8 +732,8 @@
     <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
     <col min="7" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1"/>
@@ -742,118 +754,118 @@
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
         <v>99912</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="S11" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="T11" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="U11" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="V11" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="U11" s="3" t="s">
+      <c r="W11" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -871,7 +883,7 @@
         <v>10016</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -879,13 +891,13 @@
         <v>10</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K12" s="2">
         <v>103</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M12" s="2">
         <v>-1</v>
@@ -934,7 +946,7 @@
         <v>10011</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -942,13 +954,13 @@
         <v>10</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K13" s="2">
         <v>103</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M13" s="2">
         <v>-1</v>
@@ -994,10 +1006,10 @@
         <v>70158112054</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1005,13 +1017,13 @@
         <v>14</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K14" s="2">
         <v>127</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M14" s="2">
         <v>-1</v>
@@ -1058,7 +1070,7 @@
         <v>401131</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1066,13 +1078,13 @@
         <v>14</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K15" s="2">
         <v>127</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M15" s="2">
         <v>-1</v>
@@ -1121,7 +1133,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1129,13 +1141,13 @@
         <v>10</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K16" s="2">
         <v>155</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M16" s="2">
         <v>-1</v>
@@ -1181,10 +1193,10 @@
         <v>28893419075</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1192,13 +1204,13 @@
         <v>14</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K17" s="2">
         <v>168</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M17" s="2">
         <v>-1</v>
@@ -1247,7 +1259,7 @@
         <v>1920078630</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1255,13 +1267,13 @@
         <v>10</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K18" s="2">
         <v>103</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M18" s="2">
         <v>-1</v>
@@ -1307,10 +1319,10 @@
         <v>82901123279</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1318,13 +1330,13 @@
         <v>14</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K19" s="2">
         <v>131</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M19" s="2">
         <v>-1</v>
@@ -1370,10 +1382,10 @@
         <v>82901123286</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1381,13 +1393,13 @@
         <v>14</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K20" s="2">
         <v>131</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M20" s="2">
         <v>-1</v>
@@ -1436,7 +1448,7 @@
         <v>1150</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1444,13 +1456,13 @@
         <v>10</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K21" s="2">
         <v>155</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M21" s="2">
         <v>-1</v>
@@ -1497,7 +1509,7 @@
         <v>1180</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1505,13 +1517,13 @@
         <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K22" s="2">
         <v>155</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M22" s="2">
         <v>-1</v>
@@ -1558,7 +1570,7 @@
         <v>57</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1566,13 +1578,13 @@
         <v>10</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K23" s="2">
         <v>155</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M23" s="2">
         <v>-1</v>
@@ -1621,7 +1633,7 @@
         <v>43</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1629,13 +1641,13 @@
         <v>10</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K24" s="2">
         <v>155</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M24" s="2">
         <v>-1</v>
@@ -1684,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1692,13 +1704,13 @@
         <v>10</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K25" s="2">
         <v>155</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M25" s="2">
         <v>-1</v>
@@ -1747,7 +1759,7 @@
         <v>73339</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1755,13 +1767,13 @@
         <v>10</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K26" s="2">
         <v>106</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M26" s="2">
         <v>-1</v>
@@ -1807,10 +1819,10 @@
         <v>77089150070</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1818,13 +1830,13 @@
         <v>14</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K27" s="2">
         <v>131</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M27" s="2">
         <v>-1</v>
@@ -1873,7 +1885,7 @@
         <v>3083</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1881,13 +1893,13 @@
         <v>10</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K28" s="2">
         <v>103</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M28" s="2">
         <v>-1</v>
@@ -1934,7 +1946,7 @@
         <v>2343</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1942,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K29" s="2">
         <v>-1</v>
@@ -1992,10 +2004,10 @@
         <v>23169000100</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -2003,13 +2015,13 @@
         <v>10</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K30" s="2">
         <v>155</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M30" s="2">
         <v>-1</v>
@@ -2058,7 +2070,7 @@
         <v>235159</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2066,7 +2078,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K31" s="2">
         <v>-1</v>
@@ -2116,10 +2128,10 @@
         <v>23169000070</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2127,13 +2139,13 @@
         <v>10</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K32" s="2">
         <v>155</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M32" s="2">
         <v>-1</v>
@@ -2179,10 +2191,10 @@
         <v>23169000018</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2190,13 +2202,13 @@
         <v>10</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K33" s="2">
         <v>155</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M33" s="2">
         <v>-1</v>
@@ -2242,10 +2254,10 @@
         <v>23169000193</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2253,13 +2265,13 @@
         <v>10</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K34" s="2">
         <v>155</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M34" s="2">
         <v>-1</v>
@@ -2305,10 +2317,10 @@
         <v>71626040381</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2316,13 +2328,13 @@
         <v>10</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K35" s="2">
         <v>119</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M35" s="2">
         <v>-1</v>
@@ -2369,7 +2381,7 @@
         <v>235472</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2377,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K36" s="2">
         <v>-1</v>
@@ -2427,10 +2439,10 @@
         <v>39922710223</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2438,13 +2450,13 @@
         <v>14</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K37" s="2">
         <v>129</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M37" s="2">
         <v>-1</v>
@@ -2493,7 +2505,7 @@
         <v>3200</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2501,13 +2513,13 @@
         <v>10</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K38" s="2">
         <v>155</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M38" s="2">
         <v>-1</v>
@@ -2556,7 +2568,7 @@
         <v>70000</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2564,13 +2576,13 @@
         <v>14</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K39" s="2">
         <v>143</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M39" s="2">
         <v>-1</v>
@@ -2619,7 +2631,7 @@
         <v>22102</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2627,13 +2639,13 @@
         <v>14</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K40" s="2">
         <v>143</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M40" s="2">
         <v>-1</v>
@@ -2682,7 +2694,7 @@
         <v>70312</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -2690,13 +2702,13 @@
         <v>10</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K41" s="2">
         <v>103</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M41" s="2">
         <v>-1</v>
@@ -2745,7 +2757,7 @@
         <v>70001</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -2753,13 +2765,13 @@
         <v>14</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K42" s="2">
         <v>143</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M42" s="2">
         <v>-1</v>
@@ -2808,7 +2820,7 @@
         <v>22110</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2816,13 +2828,13 @@
         <v>14</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K43" s="2">
         <v>143</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M43" s="2">
         <v>-1</v>
@@ -2871,7 +2883,7 @@
         <v>70002</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2879,13 +2891,13 @@
         <v>14</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K44" s="2">
         <v>143</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M44" s="2">
         <v>-1</v>
@@ -2934,7 +2946,7 @@
         <v>22230</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2942,13 +2954,13 @@
         <v>14</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K45" s="2">
         <v>143</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M45" s="2">
         <v>-1</v>
@@ -2994,10 +3006,10 @@
         <v>39922711121</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -3005,13 +3017,13 @@
         <v>14</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K46" s="2">
         <v>129</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M46" s="2">
         <v>-1</v>
@@ -3060,7 +3072,7 @@
         <v>70005</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3068,13 +3080,13 @@
         <v>14</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2">
         <v>143</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M47" s="2">
         <v>-1</v>
@@ -3120,10 +3132,10 @@
         <v>77089212327</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -3131,13 +3143,13 @@
         <v>14</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2">
         <v>131</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M48" s="2">
         <v>-1</v>
@@ -3183,10 +3195,10 @@
         <v>77089212334</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -3194,13 +3206,13 @@
         <v>14</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K49" s="2">
         <v>131</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M49" s="2">
         <v>-1</v>
@@ -3249,7 +3261,7 @@
         <v>22240</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -3257,13 +3269,13 @@
         <v>14</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K50" s="2">
         <v>143</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M50" s="2">
         <v>-1</v>
@@ -3312,7 +3324,7 @@
         <v>70006</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3320,13 +3332,13 @@
         <v>14</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K51" s="2">
         <v>143</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M51" s="2">
         <v>-1</v>
@@ -3375,7 +3387,7 @@
         <v>22250</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3383,13 +3395,13 @@
         <v>14</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K52" s="2">
         <v>143</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M52" s="2">
         <v>-1</v>
@@ -3438,7 +3450,7 @@
         <v>237742</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3446,7 +3458,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K53" s="2">
         <v>-1</v>
@@ -3499,7 +3511,7 @@
         <v>70007</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3507,13 +3519,13 @@
         <v>14</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K54" s="2">
         <v>143</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M54" s="2">
         <v>-1</v>
@@ -3562,7 +3574,7 @@
         <v>22300</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -3570,13 +3582,13 @@
         <v>14</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K55" s="2">
         <v>143</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M55" s="2">
         <v>-1</v>
@@ -3625,7 +3637,7 @@
         <v>70008</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -3633,13 +3645,13 @@
         <v>14</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K56" s="2">
         <v>143</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M56" s="2">
         <v>-1</v>
@@ -3688,7 +3700,7 @@
         <v>22350</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3696,13 +3708,13 @@
         <v>14</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2">
         <v>143</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M57" s="2">
         <v>-1</v>
@@ -3751,7 +3763,7 @@
         <v>70009</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3759,13 +3771,13 @@
         <v>14</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K58" s="2">
         <v>143</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M58" s="2">
         <v>-1</v>
@@ -3814,7 +3826,7 @@
         <v>22410</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -3822,13 +3834,13 @@
         <v>14</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K59" s="2">
         <v>143</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M59" s="2">
         <v>-1</v>
@@ -3877,7 +3889,7 @@
         <v>70010</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -3885,13 +3897,13 @@
         <v>14</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K60" s="2">
         <v>143</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M60" s="2">
         <v>-1</v>
@@ -3940,7 +3952,7 @@
         <v>70011</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3948,13 +3960,13 @@
         <v>14</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K61" s="2">
         <v>143</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M61" s="2">
         <v>-1</v>
@@ -4003,7 +4015,7 @@
         <v>22716</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -4011,13 +4023,13 @@
         <v>14</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K62" s="2">
         <v>143</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M62" s="2">
         <v>-1</v>
@@ -4066,7 +4078,7 @@
         <v>22718</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -4074,13 +4086,13 @@
         <v>14</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K63" s="2">
         <v>143</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M63" s="2">
         <v>-1</v>
@@ -4129,7 +4141,7 @@
         <v>70013</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -4137,13 +4149,13 @@
         <v>14</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K64" s="2">
         <v>143</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M64" s="2">
         <v>-1</v>
@@ -4192,7 +4204,7 @@
         <v>22750</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -4200,13 +4212,13 @@
         <v>14</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K65" s="2">
         <v>143</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M65" s="2">
         <v>-1</v>
@@ -4255,7 +4267,7 @@
         <v>70014</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -4263,13 +4275,13 @@
         <v>14</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K66" s="2">
         <v>143</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M66" s="2">
         <v>-1</v>
@@ -4315,10 +4327,10 @@
         <v>50139020004</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -4326,13 +4338,13 @@
         <v>10</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K67" s="2">
         <v>116</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M67" s="2">
         <v>-1</v>
@@ -4381,7 +4393,7 @@
         <v>354</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -4389,13 +4401,13 @@
         <v>14</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K68" s="2">
         <v>128</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M68" s="2">
         <v>-1</v>
@@ -4430,21 +4442,16 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{318D4D8E-7D7B-4867-9237-98FEADB44BFA}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{A0AA4BDF-D1B6-4886-AC6A-2D023E743A91}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088B14D7FA7FB0F44A0E838BCE163461C" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd631e8282ce98aa2d543c85b9ef9fd5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e4656e8c-9a70-4dea-a7e3-06aee4855942" xmlns:ns3="a056b9f5-5b41-46e9-afa5-4e72ea6cc6db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="965b20f3fb083e85ecd13ea0c8329e97" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4706,6 +4713,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4722,14 +4738,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D434FC34-B4DD-469D-A973-DE17600AD1E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B842294-CFC2-48FE-BBE5-878F02265242}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4749,6 +4757,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D434FC34-B4DD-469D-A973-DE17600AD1E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE8EC22-74BD-45B5-9AB0-5CF1C4D410A8}">
   <ds:schemaRefs>

</xml_diff>